<commit_message>
updated DCiesielski Efforts Logbook
</commit_message>
<xml_diff>
--- a/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
+++ b/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
@@ -154,16 +154,16 @@
     <t>Daniel Ciesielski</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>Made a quick webpage mockup</t>
-  </si>
-  <si>
-    <t>webpageMockup_01.pptx</t>
-  </si>
-  <si>
     <t>skypi\frontend</t>
+  </si>
+  <si>
+    <t>Requirements, webpageMockup_01.pptx</t>
+  </si>
+  <si>
+    <t>Collaborated  with team on high level plans / responsibilities, designed webpage mockup</t>
+  </si>
+  <si>
+    <t>b,d,g,n</t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -347,12 +347,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -365,24 +376,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,6 +387,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,7 +672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -675,7 +683,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -691,40 +699,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
@@ -744,162 +752,167 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:8" s="27" customFormat="1" ht="47.25">
+      <c r="A4" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="11">
-        <v>3</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26">
+        <v>4</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="18" t="s">
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" s="27" customFormat="1">
+      <c r="A5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="18" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" s="27" customFormat="1">
+      <c r="A6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="18" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" s="27" customFormat="1">
+      <c r="A7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="18" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:8" s="27" customFormat="1">
+      <c r="A8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="18" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" s="27" customFormat="1">
+      <c r="A9" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="18" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" s="27" customFormat="1">
+      <c r="A10" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="18" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+    </row>
+    <row r="11" spans="1:8" s="27" customFormat="1">
+      <c r="A11" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="18" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" s="27" customFormat="1">
+      <c r="A12" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="18" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" s="27" customFormat="1">
+      <c r="A13" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="18" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="1:8" s="27" customFormat="1">
+      <c r="A14" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="18" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="1:8" s="27" customFormat="1">
+      <c r="A15" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -913,11 +926,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -941,68 +949,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="21"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="14"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
updated ribbon.js and .css
</commit_message>
<xml_diff>
--- a/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
+++ b/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -164,6 +164,24 @@
   </si>
   <si>
     <t>b,d,g,n</t>
+  </si>
+  <si>
+    <t>a,b,c,h,i,</t>
+  </si>
+  <si>
+    <t>Worked on several tutorials for JS and React / begun implementing frontend webpage / discovered how shitty a teammate I am while sick</t>
+  </si>
+  <si>
+    <t>ribbon.js, ribbon.css</t>
+  </si>
+  <si>
+    <t>skypi\frontend\SkyPIsite</t>
+  </si>
+  <si>
+    <t>https://reactjs.org/tutorial/tutorial.html#setup-for-the-tutorial,
+https://reactjs.org/docs/create-a-new-react-app.html#create-react-app,
+inspect tool file:///C:/gitRepo/skypi/frontend/SkyPIsite/index.html
+The "Grasshopper: Learn to Code for Free" app by Area 120 on the PlayStore</t>
   </si>
 </sst>
 </file>
@@ -320,31 +338,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,6 +362,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -373,34 +392,43 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -682,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -699,215 +727,232 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="13" customFormat="1" ht="47.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="47.25">
+      <c r="A4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="12">
+      <c r="B4" s="9"/>
+      <c r="C4" s="5">
         <v>5</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:8" s="13" customFormat="1">
-      <c r="A5" s="20" t="s">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="173.25">
+      <c r="A5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:8" s="13" customFormat="1">
-      <c r="A6" s="20" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="7">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1">
+      <c r="A6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:8" s="13" customFormat="1">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" s="6" customFormat="1">
+      <c r="A7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:8" s="13" customFormat="1">
-      <c r="A8" s="20" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" s="6" customFormat="1">
+      <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8" s="13" customFormat="1">
-      <c r="A9" s="20" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" s="6" customFormat="1">
+      <c r="A9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" s="13" customFormat="1">
-      <c r="A10" s="20" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" s="6" customFormat="1">
+      <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8" s="13" customFormat="1">
-      <c r="A11" s="20" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" s="6" customFormat="1">
+      <c r="A11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:8" s="13" customFormat="1">
-      <c r="A12" s="20" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1">
+      <c r="A12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:8" s="13" customFormat="1">
-      <c r="A13" s="20" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" s="6" customFormat="1">
+      <c r="A13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:8" s="13" customFormat="1">
-      <c r="A14" s="20" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1">
+      <c r="A14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:8" s="13" customFormat="1">
-      <c r="A15" s="20" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1">
+      <c r="A15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -921,11 +966,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -935,62 +975,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="8.625" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="8.375" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="21" customWidth="1"/>
+    <col min="4" max="4" width="9" style="21" customWidth="1"/>
+    <col min="5" max="5" width="8.375" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="23"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1">
       <c r="A3" s="26"/>
@@ -1013,264 +1054,336 @@
       <c r="P3" s="27"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" ht="30.95" customHeight="1">
-      <c r="A5" s="8">
-        <v>0</v>
-      </c>
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="1:16" s="22" customFormat="1" ht="30.95" customHeight="1">
+      <c r="A5" s="28">
+        <v>0</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="28">
         <v>2</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="28">
         <v>3</v>
       </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8">
+      <c r="E5" s="30">
+        <v>1</v>
+      </c>
+      <c r="F5" s="28">
+        <v>1</v>
+      </c>
+      <c r="G5" s="28">
         <v>5</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="28">
         <v>2</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="28">
         <v>3</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="28">
         <v>2</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="28">
         <v>6</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="28">
         <v>3</v>
       </c>
-      <c r="M5" s="8">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8">
+      <c r="M5" s="28">
+        <v>1</v>
+      </c>
+      <c r="N5" s="28">
+        <v>1</v>
+      </c>
+      <c r="O5" s="28">
         <v>5</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="A6" s="31">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1">
-      <c r="A7" s="7">
+      <c r="A7" s="31">
         <v>2</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1">
-      <c r="A8" s="7">
+      <c r="A8" s="31">
         <v>3</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1">
-      <c r="A9" s="7">
+      <c r="A9" s="31">
         <v>4</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1">
-      <c r="A10" s="7">
+      <c r="A10" s="31">
         <v>5</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1">
-      <c r="A11" s="7">
+      <c r="A11" s="31">
         <v>6</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1">
-      <c r="A12" s="7">
+      <c r="A12" s="31">
         <v>7</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" ht="36" customHeight="1">
-      <c r="A13" s="7">
+      <c r="A13" s="31">
         <v>8</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="B13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Making sure my Efforts Log is up to date
</commit_message>
<xml_diff>
--- a/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
+++ b/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Team Member</t>
   </si>
   <si>
-    <t>Joe, Smith</t>
-  </si>
-  <si>
     <t>Towards objectives</t>
   </si>
   <si>
@@ -169,19 +166,22 @@
     <t>a,b,c,h,i,</t>
   </si>
   <si>
-    <t>Worked on several tutorials for JS and React / begun implementing frontend webpage / discovered how shitty a teammate I am while sick</t>
-  </si>
-  <si>
     <t>ribbon.js, ribbon.css</t>
   </si>
   <si>
     <t>skypi\frontend\SkyPIsite</t>
   </si>
   <si>
-    <t>https://reactjs.org/tutorial/tutorial.html#setup-for-the-tutorial,
-https://reactjs.org/docs/create-a-new-react-app.html#create-react-app,
+    <t>Worked on several tutorials for JS and React / begun implementing frontend webpage</t>
+  </si>
+  <si>
+    <t>https://reactjs.org/tutorial/tutorial.html#setup-for-the-tutorial
+https://reactjs.org/docs/create-a-new-react-app.html#create-react-app
 inspect tool file:///C:/gitRepo/skypi/frontend/SkyPIsite/index.html
 The "Grasshopper: Learn to Code for Free" app by Area 120 on the PlayStore</t>
+  </si>
+  <si>
+    <t>[Total]</t>
   </si>
 </sst>
 </file>
@@ -362,6 +362,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -380,55 +410,25 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -700,7 +700,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -728,11 +728,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
@@ -741,15 +741,15 @@
       <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
@@ -757,15 +757,15 @@
       <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
-      <c r="A3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="14"/>
+      <c r="A3" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="24"/>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -781,56 +781,56 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="47.25">
-      <c r="A4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="9"/>
+      <c r="A4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="19"/>
       <c r="C4" s="5">
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="173.25">
-      <c r="A5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="9"/>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="220.5">
+      <c r="A5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="19"/>
       <c r="C5" s="7">
         <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1">
-      <c r="A6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="9"/>
+      <c r="A6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
@@ -839,10 +839,10 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" s="6" customFormat="1">
-      <c r="A7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="9"/>
+      <c r="A7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="19"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
@@ -851,10 +851,10 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1">
-      <c r="A8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="9"/>
+      <c r="A8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="19"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
@@ -863,10 +863,10 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1">
-      <c r="A9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="9"/>
+      <c r="A9" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="19"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -875,10 +875,10 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1">
-      <c r="A10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="9"/>
+      <c r="A10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="19"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -887,10 +887,10 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1">
-      <c r="A11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="9"/>
+      <c r="A11" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="19"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
@@ -899,10 +899,10 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1">
-      <c r="A12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="9"/>
+      <c r="A12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="19"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
@@ -911,10 +911,10 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1">
-      <c r="A13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="9"/>
+      <c r="A13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="19"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
@@ -923,10 +923,10 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1">
-      <c r="A14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="9"/>
+      <c r="A14" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="19"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -935,10 +935,10 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1">
-      <c r="A15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="9"/>
+      <c r="A15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="19"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -948,11 +948,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -966,6 +961,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -975,190 +975,190 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="21" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9" style="21" customWidth="1"/>
-    <col min="5" max="5" width="8.375" style="21" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="21"/>
+    <col min="1" max="1" width="8.625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9" style="9" customWidth="1"/>
+    <col min="5" max="5" width="8.375" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="11" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="26"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="22" customFormat="1" ht="30.95" customHeight="1">
-      <c r="A5" s="28">
-        <v>0</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="28">
+    </row>
+    <row r="5" spans="1:16" s="10" customFormat="1" ht="30.95" customHeight="1">
+      <c r="A5" s="11">
+        <v>0</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="11">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11">
+        <v>3</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
         <v>2</v>
       </c>
-      <c r="D5" s="28">
-        <v>3</v>
-      </c>
-      <c r="E5" s="30">
-        <v>1</v>
-      </c>
-      <c r="F5" s="28">
-        <v>1</v>
-      </c>
-      <c r="G5" s="28">
-        <v>5</v>
-      </c>
-      <c r="H5" s="28">
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
         <v>2</v>
       </c>
-      <c r="I5" s="28">
-        <v>3</v>
-      </c>
-      <c r="J5" s="28">
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+      <c r="K5" s="11">
+        <v>1</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0</v>
+      </c>
+      <c r="P5" s="11">
         <v>2</v>
       </c>
-      <c r="K5" s="28">
-        <v>6</v>
-      </c>
-      <c r="L5" s="28">
-        <v>3</v>
-      </c>
-      <c r="M5" s="28">
-        <v>1</v>
-      </c>
-      <c r="N5" s="28">
-        <v>1</v>
-      </c>
-      <c r="O5" s="28">
-        <v>5</v>
-      </c>
-      <c r="P5" s="28">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1">
-      <c r="A6" s="31">
+      <c r="A6" s="14">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -1204,11 +1204,11 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1">
-      <c r="A7" s="31">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -1254,11 +1254,11 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1">
-      <c r="A8" s="31">
+      <c r="A8" s="14">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1276,11 +1276,11 @@
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1">
-      <c r="A9" s="31">
+      <c r="A9" s="14">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1298,11 +1298,11 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1">
-      <c r="A10" s="31">
+      <c r="A10" s="14">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1320,11 +1320,11 @@
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1">
-      <c r="A11" s="31">
+      <c r="A11" s="14">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1342,11 +1342,11 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1">
-      <c r="A12" s="31">
+      <c r="A12" s="14">
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1364,11 +1364,11 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" ht="36" customHeight="1">
-      <c r="A13" s="31">
+      <c r="A13" s="14">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>

</xml_diff>

<commit_message>
added Admin button to navbar
</commit_message>
<xml_diff>
--- a/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
+++ b/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -182,6 +182,10 @@
   </si>
   <si>
     <t>[Total]</t>
+  </si>
+  <si>
+    <t>created stations page foundation,
+admin button</t>
   </si>
 </sst>
 </file>
@@ -380,6 +384,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -390,24 +412,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -700,7 +704,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -711,7 +715,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -727,40 +731,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -781,10 +785,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="47.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="5">
         <v>5</v>
       </c>
@@ -803,10 +807,10 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" ht="220.5">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="7">
         <v>15</v>
       </c>
@@ -827,10 +831,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" s="6" customFormat="1">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
@@ -838,23 +842,27 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="31.5">
+      <c r="A7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="7">
+        <v>8</v>
+      </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
@@ -863,10 +871,10 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -875,10 +883,10 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -887,10 +895,10 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
@@ -899,10 +907,10 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
@@ -911,10 +919,10 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
@@ -923,10 +931,10 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -935,10 +943,10 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -948,6 +956,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -961,11 +974,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made stations sizing similar to dashboard
</commit_message>
<xml_diff>
--- a/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
+++ b/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Objectives</t>
   </si>
   <si>
-    <t>Example Template</t>
-  </si>
-  <si>
     <t>Your Name</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>Sprint # 12</t>
-  </si>
-  <si>
-    <t>Example Project</t>
   </si>
   <si>
     <t>Daniel Ciesielski</t>
@@ -186,6 +180,24 @@
   <si>
     <t>created stations page foundation,
 admin button</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=A71aqufiNtQ</t>
+  </si>
+  <si>
+    <t>dashboard.js
+login.js
+projectmanager</t>
+  </si>
+  <si>
+    <t>skypi\fronted\client\src
+sprint03\projectmanager</t>
+  </si>
+  <si>
+    <t>Worked on more tutorials, helped build dashboard page, helped build login page, meet with sponser</t>
+  </si>
+  <si>
+    <t>SkyPi</t>
   </si>
 </sst>
 </file>
@@ -342,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -377,9 +389,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -714,7 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -731,40 +740,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1">
-      <c r="A3" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="20"/>
+      <c r="A3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="19"/>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -785,84 +794,94 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" ht="47.25">
-      <c r="A4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="15"/>
+      <c r="A4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="14"/>
       <c r="C4" s="5">
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" s="6" customFormat="1" ht="220.5">
-      <c r="A5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="15"/>
+      <c r="A5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="14"/>
       <c r="C5" s="7">
         <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="6" customFormat="1">
-      <c r="A6" s="15" t="s">
+    </row>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="78.75">
+      <c r="A6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="7">
+        <v>20</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="31.5">
+      <c r="A7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="31.5">
-      <c r="A7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="7">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" s="6" customFormat="1">
-      <c r="A8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="15"/>
+      <c r="A8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="14"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
@@ -871,10 +890,10 @@
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1">
-      <c r="A9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="15"/>
+      <c r="A9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="14"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -883,10 +902,10 @@
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1">
-      <c r="A10" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="15"/>
+      <c r="A10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="14"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -895,10 +914,10 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1">
-      <c r="A11" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="15"/>
+      <c r="A11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="14"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8"/>
@@ -907,10 +926,10 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1">
-      <c r="A12" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="15"/>
+      <c r="A12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="14"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
@@ -919,10 +938,10 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1">
-      <c r="A13" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="15"/>
+      <c r="A13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="14"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
@@ -931,10 +950,10 @@
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1">
-      <c r="A14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="15"/>
+      <c r="A14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="14"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -943,10 +962,10 @@
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1">
-      <c r="A15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="15"/>
+      <c r="A15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="14"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -983,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -998,72 +1017,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="26"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -1116,113 +1135,127 @@
         <v>0</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="11">
-        <v>1</v>
+        <f>SUM(C6:C13)</f>
+        <v>2</v>
       </c>
       <c r="D5" s="11">
+        <f t="shared" ref="D5:P5" si="0">SUM(D6:D13)</f>
         <v>3</v>
       </c>
-      <c r="E5" s="13">
-        <v>1</v>
+      <c r="E5" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11">
-        <v>0</v>
-      </c>
-      <c r="I5" s="11">
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J5" s="11">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11">
-        <v>1</v>
-      </c>
       <c r="L5" s="11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="M5" s="11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="N5" s="11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O5" s="11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P5" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="36" customHeight="1">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="36" customHeight="1">
+      <c r="A7" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="36" customHeight="1">
-      <c r="A6" s="14">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="36" customHeight="1">
-      <c r="A7" s="14">
-        <v>2</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -1262,39 +1295,69 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -1303,14 +1366,16 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
+      <c r="P9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1328,11 +1393,11 @@
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1350,11 +1415,11 @@
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1372,11 +1437,11 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" ht="36" customHeight="1">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>

</xml_diff>

<commit_message>
changed delete modal text color
</commit_message>
<xml_diff>
--- a/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
+++ b/docs/logbooks/DCiesielski - Efforts Logbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1575" yWindow="3195" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -178,10 +178,6 @@
     <t>[Total]</t>
   </si>
   <si>
-    <t>created stations page foundation,
-admin button</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=A71aqufiNtQ</t>
   </si>
   <si>
@@ -198,6 +194,45 @@
   </si>
   <si>
     <t>SkyPi</t>
+  </si>
+  <si>
+    <t>skypi\frontend\client\src\components\layout
+skypi\frontend\client\src\components\content\user
+..\stations
+..\dashboard
+..\admin</t>
+  </si>
+  <si>
+    <t>LogoutModal.js
+Navbar.js
+DeleteModal.js
+Stations.js
+Dashboard.js
+Timegraph.js
+AdminPage.js</t>
+  </si>
+  <si>
+    <t>created stations page,
+admin button / page foundations,
+dashboard chart,
+stations favorite buttons</t>
+  </si>
+  <si>
+    <t>Navbar.js
+Stations.js
+Dashboard.js
+Timegraph.js
+AdminPage.js</t>
+  </si>
+  <si>
+    <t>logout modal,
+delete profile modal,
+dashboard charts,
+stations favorite buttons</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/react-modal
+https://www.w3schools.com/cssref/pr_class_position.asp</t>
   </si>
 </sst>
 </file>
@@ -723,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -759,7 +794,7 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
@@ -849,45 +884,59 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="H6" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="31.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="157.5">
       <c r="A7" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="7">
-        <v>8.5</v>
+        <v>30</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+        <v>57</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="157.5">
       <c r="A8" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7">
+        <v>42</v>
+      </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:8" s="6" customFormat="1">
       <c r="A9" s="14" t="s">
@@ -1002,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1044,7 +1093,7 @@
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="26"/>
       <c r="E2" s="26"/>
@@ -1139,55 +1188,55 @@
       </c>
       <c r="C5" s="11">
         <f>SUM(C6:C13)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" ref="D5:P5" si="0">SUM(D6:D13)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5" s="11">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J5" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K5" s="11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L5" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N5" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P5" s="11">
         <f t="shared" si="0"/>
@@ -1351,21 +1400,45 @@
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
       <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
       <c r="P9" s="3">
         <v>1</v>
       </c>
@@ -1377,20 +1450,48 @@
       <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1">
       <c r="A11" s="13">

</xml_diff>